<commit_message>
added impedance analyzer files
</commit_message>
<xml_diff>
--- a/5-16-12/testing_data.xlsx
+++ b/5-16-12/testing_data.xlsx
@@ -4,14 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="600" windowWidth="25040" windowHeight="17820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -22,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>2-pk2pk</t>
   </si>
@@ -51,7 +48,22 @@
     <t>Current going through the resistive load</t>
   </si>
   <si>
-    <t>11:52AM</t>
+    <t>12:07PM</t>
+  </si>
+  <si>
+    <t>12:28PM</t>
+  </si>
+  <si>
+    <t>12:56PM</t>
+  </si>
+  <si>
+    <t>1:16PM</t>
+  </si>
+  <si>
+    <t>3:23PM</t>
+  </si>
+  <si>
+    <t>1:42PM</t>
   </si>
 </sst>
 </file>
@@ -179,50 +191,47 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$18</c:f>
+              <c:f>Sheet1!$C$5:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>450.0</c:v>
+                  <c:v>428.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>451.0</c:v>
+                  <c:v>429.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>452.0</c:v>
+                  <c:v>429.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>453.0</c:v>
+                  <c:v>429.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>454.0</c:v>
+                  <c:v>429.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>455.0</c:v>
+                  <c:v>429.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>456.0</c:v>
+                  <c:v>457.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>457.0</c:v>
+                  <c:v>458.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>458.0</c:v>
+                  <c:v>459.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>459.0</c:v>
+                  <c:v>460.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>460.0</c:v>
+                  <c:v>461.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>461.0</c:v>
+                  <c:v>462.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>462.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>463.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -238,50 +247,47 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$18</c:f>
+              <c:f>Sheet1!$D$5:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>438.0</c:v>
+                  <c:v>417.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>439.0</c:v>
+                  <c:v>417.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>440.0</c:v>
+                  <c:v>417.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>441.0</c:v>
+                  <c:v>417.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>442.0</c:v>
+                  <c:v>417.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>443.0</c:v>
+                  <c:v>417.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>444.0</c:v>
+                  <c:v>445.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>445.0</c:v>
+                  <c:v>446.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>446.0</c:v>
+                  <c:v>447.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>447.0</c:v>
+                  <c:v>448.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>448.0</c:v>
+                  <c:v>449.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>449.0</c:v>
+                  <c:v>450.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>450.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>451.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -299,11 +305,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="552965848"/>
-        <c:axId val="552876808"/>
+        <c:axId val="494108904"/>
+        <c:axId val="4082552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="552965848"/>
+        <c:axId val="494108904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -331,7 +337,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="552876808"/>
+        <c:crossAx val="4082552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -339,7 +345,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="552876808"/>
+        <c:axId val="4082552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -373,7 +379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="552965848"/>
+        <c:crossAx val="494108904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -452,50 +458,47 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$18</c:f>
+              <c:f>Sheet1!$E$5:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>5.09</c:v>
+                  <c:v>5.093</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1</c:v>
+                  <c:v>5.093</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.11</c:v>
+                  <c:v>5.093</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.12</c:v>
+                  <c:v>5.093</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.13</c:v>
+                  <c:v>5.093</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.14</c:v>
+                  <c:v>5.092</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.15</c:v>
+                  <c:v>5.16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.16</c:v>
+                  <c:v>5.17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.17</c:v>
+                  <c:v>5.18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.18</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.19</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.2</c:v>
+                  <c:v>5.21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.21</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>5.22</c:v>
                 </c:pt>
               </c:numCache>
@@ -511,50 +514,47 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$5:$F$18</c:f>
+              <c:f>Sheet1!$F$5:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>5.08</c:v>
+                  <c:v>5.089</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.09</c:v>
+                  <c:v>5.089</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1</c:v>
+                  <c:v>5.088</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.11</c:v>
+                  <c:v>5.0886</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.12</c:v>
+                  <c:v>5.0886</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.13</c:v>
+                  <c:v>5.0875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.14</c:v>
+                  <c:v>5.15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.15</c:v>
+                  <c:v>5.16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.16</c:v>
+                  <c:v>5.17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.17</c:v>
+                  <c:v>5.18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.18</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.19</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>5.21</c:v>
                 </c:pt>
               </c:numCache>
@@ -572,11 +572,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="563103992"/>
-        <c:axId val="563557096"/>
+        <c:axId val="494174152"/>
+        <c:axId val="494179864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="563103992"/>
+        <c:axId val="494174152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,7 +609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="563557096"/>
+        <c:crossAx val="494179864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -617,7 +617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="563557096"/>
+        <c:axId val="494179864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,7 +647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="563103992"/>
+        <c:crossAx val="494174152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -716,50 +716,47 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$5:$G$18</c:f>
+              <c:f>Sheet1!$G$5:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>108.2978723404255</c:v>
+                  <c:v>108.3617021276596</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108.5106382978723</c:v>
+                  <c:v>108.3617021276596</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108.7234042553192</c:v>
+                  <c:v>108.3617021276596</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108.936170212766</c:v>
+                  <c:v>108.3617021276596</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>109.1489361702128</c:v>
+                  <c:v>108.3617021276596</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>109.3617021276596</c:v>
+                  <c:v>108.3404255319149</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>109.5744680851064</c:v>
+                  <c:v>109.7872340425532</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>109.7872340425532</c:v>
+                  <c:v>110.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110.0</c:v>
+                  <c:v>110.2127659574468</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>110.2127659574468</c:v>
+                  <c:v>110.4255319148936</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>110.4255319148936</c:v>
+                  <c:v>110.6382978723404</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110.6382978723404</c:v>
+                  <c:v>110.8510638297872</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>110.8510638297872</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>111.063829787234</c:v>
                 </c:pt>
               </c:numCache>
@@ -775,50 +772,47 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$5:$H$18</c:f>
+              <c:f>Sheet1!$H$5:$H$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>108.0851063829787</c:v>
+                  <c:v>108.2765957446809</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108.2978723404255</c:v>
+                  <c:v>108.2765957446809</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108.5106382978723</c:v>
+                  <c:v>108.2553191489362</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108.7234042553192</c:v>
+                  <c:v>108.268085106383</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108.936170212766</c:v>
+                  <c:v>108.268085106383</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>109.1489361702128</c:v>
+                  <c:v>108.2446808510638</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>109.3617021276596</c:v>
+                  <c:v>109.5744680851064</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>109.5744680851064</c:v>
+                  <c:v>109.7872340425532</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>109.7872340425532</c:v>
+                  <c:v>110.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>110.0</c:v>
+                  <c:v>110.2127659574468</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>110.2127659574468</c:v>
+                  <c:v>110.4255319148936</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110.4255319148936</c:v>
+                  <c:v>110.6382978723404</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>110.6382978723404</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>110.8510638297872</c:v>
                 </c:pt>
               </c:numCache>
@@ -836,11 +830,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="551312424"/>
-        <c:axId val="551452104"/>
+        <c:axId val="480578616"/>
+        <c:axId val="480584104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="551312424"/>
+        <c:axId val="480578616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,7 +862,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551452104"/>
+        <c:crossAx val="480584104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -876,7 +870,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551452104"/>
+        <c:axId val="480584104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,7 +900,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551312424"/>
+        <c:crossAx val="480578616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -940,7 +934,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -966,13 +960,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1004,7 +998,7 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1027,240 +1021,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="9">
-          <cell r="C9">
-            <v>0.33700000000000002</v>
-          </cell>
-          <cell r="D9">
-            <v>0.48</v>
-          </cell>
-          <cell r="E9">
-            <v>5.069</v>
-          </cell>
-          <cell r="F9">
-            <v>5.0620000000000003</v>
-          </cell>
-          <cell r="G9">
-            <v>50.69</v>
-          </cell>
-          <cell r="H9">
-            <v>50.620000000000005</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>0.33600000000000002</v>
-          </cell>
-          <cell r="D10">
-            <v>0.46500000000000002</v>
-          </cell>
-          <cell r="E10">
-            <v>5.0780000000000003</v>
-          </cell>
-          <cell r="F10">
-            <v>5.0720000000000001</v>
-          </cell>
-          <cell r="G10">
-            <v>50.780000000000008</v>
-          </cell>
-          <cell r="H10">
-            <v>50.72</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>0.33600000000000002</v>
-          </cell>
-          <cell r="D11">
-            <v>0.46500000000000002</v>
-          </cell>
-          <cell r="E11">
-            <v>5.0789999999999997</v>
-          </cell>
-          <cell r="F11">
-            <v>5.0720000000000001</v>
-          </cell>
-          <cell r="G11">
-            <v>50.789999999999992</v>
-          </cell>
-          <cell r="H11">
-            <v>50.72</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>0.33700000000000002</v>
-          </cell>
-          <cell r="D12">
-            <v>0.41099999999999998</v>
-          </cell>
-          <cell r="E12">
-            <v>5.0860000000000003</v>
-          </cell>
-          <cell r="F12">
-            <v>5.085</v>
-          </cell>
-          <cell r="G12">
-            <v>50.86</v>
-          </cell>
-          <cell r="H12">
-            <v>50.85</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>0.33800000000000002</v>
-          </cell>
-          <cell r="D13">
-            <v>0.40899999999999997</v>
-          </cell>
-          <cell r="E13">
-            <v>5.0810000000000004</v>
-          </cell>
-          <cell r="F13">
-            <v>5.0830000000000002</v>
-          </cell>
-          <cell r="G13">
-            <v>50.81</v>
-          </cell>
-          <cell r="H13">
-            <v>50.83</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>0.33800000000000002</v>
-          </cell>
-          <cell r="D14">
-            <v>0.41599999999999998</v>
-          </cell>
-          <cell r="E14">
-            <v>5.1040000000000001</v>
-          </cell>
-          <cell r="F14">
-            <v>5.1050000000000004</v>
-          </cell>
-          <cell r="G14">
-            <v>51.04</v>
-          </cell>
-          <cell r="H14">
-            <v>51.050000000000004</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>0.33500000000000002</v>
-          </cell>
-          <cell r="D15">
-            <v>0.41099999999999998</v>
-          </cell>
-          <cell r="E15">
-            <v>5.101</v>
-          </cell>
-          <cell r="F15">
-            <v>5.101</v>
-          </cell>
-          <cell r="G15">
-            <v>51.01</v>
-          </cell>
-          <cell r="H15">
-            <v>51.01</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>0.33700000000000002</v>
-          </cell>
-          <cell r="D16">
-            <v>0.41099999999999998</v>
-          </cell>
-          <cell r="E16">
-            <v>5.0910000000000002</v>
-          </cell>
-          <cell r="F16">
-            <v>5.0940000000000003</v>
-          </cell>
-          <cell r="G16">
-            <v>50.910000000000004</v>
-          </cell>
-          <cell r="H16">
-            <v>50.940000000000005</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>0.33700000000000002</v>
-          </cell>
-          <cell r="D17">
-            <v>0.41099999999999998</v>
-          </cell>
-          <cell r="E17">
-            <v>5.0940000000000003</v>
-          </cell>
-          <cell r="F17">
-            <v>5.0960000000000001</v>
-          </cell>
-          <cell r="G17">
-            <v>50.940000000000005</v>
-          </cell>
-          <cell r="H17">
-            <v>50.96</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>0.33800000000000002</v>
-          </cell>
-          <cell r="D18">
-            <v>0.41</v>
-          </cell>
-          <cell r="E18">
-            <v>5.093</v>
-          </cell>
-          <cell r="F18">
-            <v>5.0949999999999998</v>
-          </cell>
-          <cell r="G18">
-            <v>50.93</v>
-          </cell>
-          <cell r="H18">
-            <v>50.949999999999996</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>0.33800000000000002</v>
-          </cell>
-          <cell r="D19">
-            <v>0.41</v>
-          </cell>
-          <cell r="E19">
-            <v>5.1020000000000003</v>
-          </cell>
-          <cell r="F19">
-            <v>5.1040000000000001</v>
-          </cell>
-          <cell r="G19">
-            <v>51.02</v>
-          </cell>
-          <cell r="H19">
-            <v>51.04</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1585,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A18"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1635,333 +1395,321 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="C5">
-        <v>450</v>
+        <v>428</v>
       </c>
       <c r="D5">
-        <v>438</v>
+        <v>417</v>
       </c>
       <c r="E5">
-        <v>5.09</v>
+        <v>5.093</v>
       </c>
       <c r="F5">
-        <v>5.08</v>
+        <v>5.0890000000000004</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:H15" si="0">E5/$I$2*1000</f>
-        <v>108.29787234042553</v>
+        <f t="shared" ref="G5:G17" si="0">E5/$I$2*1000</f>
+        <v>108.36170212765957</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
-        <v>108.08510638297872</v>
+        <f t="shared" ref="H5:H17" si="1">F5/$I$2*1000</f>
+        <v>108.27659574468086</v>
       </c>
     </row>
     <row r="6" spans="1:9">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C6">
-        <v>451</v>
+        <v>429</v>
       </c>
       <c r="D6">
-        <v>439</v>
+        <v>417.6</v>
       </c>
       <c r="E6">
-        <v>5.0999999999999996</v>
+        <v>5.093</v>
       </c>
       <c r="F6">
-        <v>5.09</v>
+        <v>5.0890000000000004</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G18" si="1">E6/$I$2*1000</f>
-        <v>108.51063829787233</v>
+        <f t="shared" si="0"/>
+        <v>108.36170212765957</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H18" si="2">F6/$I$2*1000</f>
-        <v>108.29787234042553</v>
+        <f t="shared" si="1"/>
+        <v>108.27659574468086</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C7">
-        <v>452</v>
+        <v>429.5</v>
       </c>
       <c r="D7">
-        <v>440</v>
+        <v>417.8</v>
       </c>
       <c r="E7">
-        <v>5.1100000000000003</v>
+        <v>5.093</v>
       </c>
       <c r="F7">
-        <v>5.0999999999999996</v>
+        <v>5.0880000000000001</v>
       </c>
       <c r="G7">
+        <f t="shared" si="0"/>
+        <v>108.36170212765957</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="1"/>
-        <v>108.72340425531915</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="2"/>
-        <v>108.51063829787233</v>
+        <v>108.25531914893617</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="C8">
-        <v>453</v>
+        <v>429.7</v>
       </c>
       <c r="D8">
-        <v>441</v>
+        <v>417.7</v>
       </c>
       <c r="E8">
-        <v>5.12</v>
+        <v>5.093</v>
       </c>
       <c r="F8">
-        <v>5.1100000000000003</v>
+        <v>5.0885999999999996</v>
       </c>
       <c r="G8">
+        <f t="shared" si="0"/>
+        <v>108.36170212765957</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="1"/>
-        <v>108.93617021276596</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="2"/>
-        <v>108.72340425531915</v>
+        <v>108.26808510638297</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="C9">
-        <v>454</v>
+        <v>429.5</v>
       </c>
       <c r="D9">
-        <v>442</v>
+        <v>417.5</v>
       </c>
       <c r="E9">
-        <v>5.13</v>
+        <v>5.093</v>
       </c>
       <c r="F9">
-        <v>5.12</v>
+        <v>5.0885999999999996</v>
       </c>
       <c r="G9">
+        <f t="shared" si="0"/>
+        <v>108.36170212765957</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="1"/>
-        <v>109.14893617021276</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
-        <v>108.93617021276596</v>
+        <v>108.26808510638297</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="C10">
-        <v>455</v>
+        <v>429.4</v>
       </c>
       <c r="D10">
-        <v>443</v>
+        <v>417.5</v>
       </c>
       <c r="E10">
-        <v>5.14</v>
+        <v>5.0919999999999996</v>
       </c>
       <c r="F10">
-        <v>5.13</v>
+        <v>5.0875000000000004</v>
       </c>
       <c r="G10">
+        <f t="shared" si="0"/>
+        <v>108.34042553191489</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="1"/>
-        <v>109.36170212765957</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
-        <v>109.14893617021276</v>
+        <v>108.24468085106383</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2"/>
       <c r="C11">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D11">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E11">
+        <v>5.16</v>
+      </c>
+      <c r="F11">
         <v>5.15</v>
       </c>
-      <c r="F11">
-        <v>5.14</v>
-      </c>
       <c r="G11">
+        <f t="shared" si="0"/>
+        <v>109.78723404255319</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="1"/>
         <v>109.57446808510639</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
-        <v>109.36170212765957</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2"/>
       <c r="C12">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D12">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="E12">
+        <v>5.17</v>
+      </c>
+      <c r="F12">
         <v>5.16</v>
       </c>
-      <c r="F12">
-        <v>5.15</v>
-      </c>
       <c r="G12">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="1"/>
         <v>109.78723404255319</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
-        <v>109.57446808510639</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2"/>
       <c r="C13">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D13">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="E13">
+        <v>5.18</v>
+      </c>
+      <c r="F13">
         <v>5.17</v>
       </c>
-      <c r="F13">
-        <v>5.16</v>
-      </c>
       <c r="G13">
+        <f t="shared" si="0"/>
+        <v>110.21276595744681</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="1"/>
         <v>110</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
-        <v>109.78723404255319</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2"/>
       <c r="C14">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D14">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E14">
+        <v>5.19</v>
+      </c>
+      <c r="F14">
         <v>5.18</v>
       </c>
-      <c r="F14">
-        <v>5.17</v>
-      </c>
       <c r="G14">
+        <f t="shared" si="0"/>
+        <v>110.42553191489363</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="1"/>
         <v>110.21276595744681</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="2"/>
-        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2"/>
       <c r="C15">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D15">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E15">
+        <v>5.2</v>
+      </c>
+      <c r="F15">
         <v>5.19</v>
       </c>
-      <c r="F15">
-        <v>5.18</v>
-      </c>
       <c r="G15">
+        <f t="shared" si="0"/>
+        <v>110.63829787234043</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="1"/>
         <v>110.42553191489363</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>110.21276595744681</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2"/>
       <c r="C16">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D16">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E16">
+        <v>5.21</v>
+      </c>
+      <c r="F16">
         <v>5.2</v>
       </c>
-      <c r="F16">
-        <v>5.19</v>
-      </c>
       <c r="G16">
+        <f t="shared" si="0"/>
+        <v>110.85106382978724</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="1"/>
         <v>110.63829787234043</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="2"/>
-        <v>110.42553191489363</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2"/>
       <c r="C17">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D17">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E17">
+        <v>5.22</v>
+      </c>
+      <c r="F17">
         <v>5.21</v>
       </c>
-      <c r="F17">
-        <v>5.2</v>
-      </c>
       <c r="G17">
+        <f t="shared" si="0"/>
+        <v>111.06382978723403</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="1"/>
         <v>110.85106382978724</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="2"/>
-        <v>110.63829787234043</v>
-      </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="2"/>
-      <c r="C18">
-        <v>463</v>
-      </c>
-      <c r="D18">
-        <v>451</v>
-      </c>
-      <c r="E18">
-        <v>5.22</v>
-      </c>
-      <c r="F18">
-        <v>5.21</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="1"/>
-        <v>111.06382978723403</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="2"/>
-        <v>110.85106382978724</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
+      <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C18" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adedd new data for capacitors
</commit_message>
<xml_diff>
--- a/5-16-12/testing_data.xlsx
+++ b/5-16-12/testing_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>2-pk2pk</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t>7:43PM</t>
+  </si>
+  <si>
+    <t>8:29PM</t>
+  </si>
+  <si>
+    <t>9:11PM</t>
+  </si>
+  <si>
+    <t>9:38PM</t>
+  </si>
+  <si>
+    <t>9:54PM</t>
   </si>
 </sst>
 </file>
@@ -252,13 +264,13 @@
                   <c:v>434.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>434.6</c:v>
+                  <c:v>434.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>434.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>434.6</c:v>
+                  <c:v>435.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -299,7 +311,7 @@
                   <c:v>396.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>396.3</c:v>
+                  <c:v>396.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -486,16 +498,16 @@
                   <c:v>4.9784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9784</c:v>
+                  <c:v>4.9783</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9784</c:v>
+                  <c:v>4.9785</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9784</c:v>
+                  <c:v>4.9789</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9784</c:v>
+                  <c:v>4.9786</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -527,16 +539,16 @@
                   <c:v>4.9808</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9808</c:v>
+                  <c:v>4.981</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9808</c:v>
+                  <c:v>4.981</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9808</c:v>
+                  <c:v>4.9812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9808</c:v>
+                  <c:v>4.9809</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -714,16 +726,16 @@
                   <c:v>105.9234042553191</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105.9234042553191</c:v>
+                  <c:v>105.9212765957447</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105.9234042553191</c:v>
+                  <c:v>105.9255319148936</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105.9234042553191</c:v>
+                  <c:v>105.9340425531915</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>105.9234042553191</c:v>
+                  <c:v>105.9276595744681</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -755,16 +767,16 @@
                   <c:v>105.9744680851064</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105.9744680851064</c:v>
+                  <c:v>105.9787234042553</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105.9744680851064</c:v>
+                  <c:v>105.9787234042553</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105.9744680851064</c:v>
+                  <c:v>105.9829787234043</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>105.9744680851064</c:v>
+                  <c:v>105.9765957446808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -940,13 +952,13 @@
                   <c:v>434.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>434.6</c:v>
+                  <c:v>434.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>434.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>434.6</c:v>
+                  <c:v>435.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -987,7 +999,7 @@
                   <c:v>396.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>396.3</c:v>
+                  <c:v>396.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1174,16 +1186,16 @@
                   <c:v>4.9784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9784</c:v>
+                  <c:v>4.9783</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9784</c:v>
+                  <c:v>4.9785</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9784</c:v>
+                  <c:v>4.9789</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9784</c:v>
+                  <c:v>4.9786</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1215,16 +1227,16 @@
                   <c:v>4.9808</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9808</c:v>
+                  <c:v>4.981</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9808</c:v>
+                  <c:v>4.981</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9808</c:v>
+                  <c:v>4.9812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9808</c:v>
+                  <c:v>4.9809</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1402,16 +1414,16 @@
                   <c:v>105.9234042553191</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105.9234042553191</c:v>
+                  <c:v>105.9212765957447</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105.9234042553191</c:v>
+                  <c:v>105.9255319148936</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105.9234042553191</c:v>
+                  <c:v>105.9340425531915</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>105.9234042553191</c:v>
+                  <c:v>105.9276595744681</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1443,16 +1455,16 @@
                   <c:v>105.9744680851064</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105.9744680851064</c:v>
+                  <c:v>105.9787234042553</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105.9744680851064</c:v>
+                  <c:v>105.9787234042553</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105.9744680851064</c:v>
+                  <c:v>105.9829787234043</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>105.9744680851064</c:v>
+                  <c:v>105.9765957446808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2088,7 +2100,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:F16"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2235,7 +2247,9 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="C9">
         <v>434.6</v>
       </c>
@@ -2243,45 +2257,49 @@
         <v>396.3</v>
       </c>
       <c r="E9">
-        <v>4.9783999999999997</v>
+        <v>4.9782999999999999</v>
       </c>
       <c r="F9">
-        <v>4.9808000000000003</v>
+        <v>4.9809999999999999</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>105.92340425531914</v>
+        <v>105.92127659574469</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>105.97446808510639</v>
+        <v>105.97872340425532</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="C10">
-        <v>434.6</v>
+        <v>434.8</v>
       </c>
       <c r="D10">
         <v>396.3</v>
       </c>
       <c r="E10">
-        <v>4.9783999999999997</v>
+        <v>4.9785000000000004</v>
       </c>
       <c r="F10">
-        <v>4.9808000000000003</v>
+        <v>4.9809999999999999</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>105.92340425531914</v>
+        <v>105.92553191489363</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>105.97446808510639</v>
+        <v>105.97872340425532</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C11">
         <v>434.6</v>
       </c>
@@ -2289,133 +2307,87 @@
         <v>396.3</v>
       </c>
       <c r="E11">
-        <v>4.9783999999999997</v>
+        <v>4.9789000000000003</v>
       </c>
       <c r="F11">
-        <v>4.9808000000000003</v>
+        <v>4.9812000000000003</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>105.92340425531914</v>
+        <v>105.9340425531915</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>105.97446808510639</v>
+        <v>105.98297872340426</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C12">
-        <v>434.6</v>
+        <v>435</v>
       </c>
       <c r="D12">
-        <v>396.3</v>
+        <v>396.7</v>
       </c>
       <c r="E12">
-        <v>4.9783999999999997</v>
+        <v>4.9786000000000001</v>
       </c>
       <c r="F12">
-        <v>4.9808000000000003</v>
+        <v>4.9809000000000001</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>105.92340425531914</v>
+        <v>105.92765957446809</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>105.97446808510639</v>
+        <v>105.97659574468085</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2"/>
-      <c r="C13">
-        <v>434.6</v>
-      </c>
-      <c r="D13">
-        <v>396.3</v>
-      </c>
-      <c r="E13">
-        <v>4.9783999999999997</v>
-      </c>
-      <c r="F13">
-        <v>4.9808000000000003</v>
-      </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>105.92340425531914</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>105.97446808510639</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2"/>
-      <c r="C14">
-        <v>434.6</v>
-      </c>
-      <c r="D14">
-        <v>396.3</v>
-      </c>
-      <c r="E14">
-        <v>4.9783999999999997</v>
-      </c>
-      <c r="F14">
-        <v>4.9808000000000003</v>
-      </c>
       <c r="G14">
         <f t="shared" ref="G14:G16" si="2">E14/$I$2*1000</f>
-        <v>105.92340425531914</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <f t="shared" ref="H14:H16" si="3">F14/$I$2*1000</f>
-        <v>105.97446808510639</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2"/>
-      <c r="C15">
-        <v>434.6</v>
-      </c>
-      <c r="D15">
-        <v>396.3</v>
-      </c>
-      <c r="E15">
-        <v>4.9783999999999997</v>
-      </c>
-      <c r="F15">
-        <v>4.9808000000000003</v>
-      </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>105.92340425531914</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <f t="shared" si="3"/>
-        <v>105.97446808510639</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2"/>
-      <c r="C16">
-        <v>434.6</v>
-      </c>
-      <c r="D16">
-        <v>396.3</v>
-      </c>
-      <c r="E16">
-        <v>4.9783999999999997</v>
-      </c>
-      <c r="F16">
-        <v>4.9808000000000003</v>
-      </c>
       <c r="G16">
         <f t="shared" si="2"/>
-        <v>105.92340425531914</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <f t="shared" si="3"/>
-        <v>105.97446808510639</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">

</xml_diff>